<commit_message>
commited how it works
</commit_message>
<xml_diff>
--- a/food production.xlsx
+++ b/food production.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashis ray\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashis ray\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{324BB054-F6C3-4BC7-B5CB-964721F75D56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F3ACF8F-2490-4DF0-AC2A-D7AD43009F94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{298ADBC1-6D3C-44E6-A5B7-CAAEA5ABB211}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="32">
   <si>
     <t>Date</t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>Food Production(in million metric tons)</t>
+  </si>
+  <si>
+    <t>Jammu and Kashmir</t>
   </si>
 </sst>
 </file>
@@ -472,8 +475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{597E5987-E992-4582-9D2C-48A61452FC6A}">
   <dimension ref="A1:C146"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C137" sqref="C137"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -994,10 +997,10 @@
         <v>44197</v>
       </c>
       <c r="B47" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="C47">
-        <v>0.89</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
@@ -1005,10 +1008,10 @@
         <v>44228</v>
       </c>
       <c r="B48" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="C48">
-        <v>0.92</v>
+        <v>0.49</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
@@ -1016,10 +1019,10 @@
         <v>44256</v>
       </c>
       <c r="B49" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="C49">
-        <v>0.91</v>
+        <v>0.49</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
@@ -1027,10 +1030,10 @@
         <v>44287</v>
       </c>
       <c r="B50" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="C50">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
@@ -1038,10 +1041,10 @@
         <v>44317</v>
       </c>
       <c r="B51" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="C51">
-        <v>0.92</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
@@ -1049,10 +1052,10 @@
         <v>44197</v>
       </c>
       <c r="B52" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C52">
-        <v>0.81</v>
+        <v>0.89</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
@@ -1060,10 +1063,10 @@
         <v>44228</v>
       </c>
       <c r="B53" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C53">
-        <v>0.83</v>
+        <v>0.92</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
@@ -1071,10 +1074,10 @@
         <v>44256</v>
       </c>
       <c r="B54" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C54">
-        <v>0.82</v>
+        <v>0.91</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
@@ -1082,10 +1085,10 @@
         <v>44287</v>
       </c>
       <c r="B55" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C55">
-        <v>0.79</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
@@ -1093,10 +1096,10 @@
         <v>44317</v>
       </c>
       <c r="B56" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C56">
-        <v>0.85</v>
+        <v>0.92</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
@@ -1104,10 +1107,10 @@
         <v>44197</v>
       </c>
       <c r="B57" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C57">
-        <v>0.46</v>
+        <v>0.81</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
@@ -1115,10 +1118,10 @@
         <v>44228</v>
       </c>
       <c r="B58" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C58">
-        <v>0.48</v>
+        <v>0.83</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
@@ -1126,10 +1129,10 @@
         <v>44256</v>
       </c>
       <c r="B59" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C59">
-        <v>0.48</v>
+        <v>0.82</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
@@ -1137,10 +1140,10 @@
         <v>44287</v>
       </c>
       <c r="B60" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C60">
-        <v>0.5</v>
+        <v>0.79</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
@@ -1148,10 +1151,10 @@
         <v>44317</v>
       </c>
       <c r="B61" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C61">
-        <v>0.48</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
@@ -1159,10 +1162,10 @@
         <v>44197</v>
       </c>
       <c r="B62" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C62">
-        <v>2.4900000000000002</v>
+        <v>0.46</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
@@ -1170,10 +1173,10 @@
         <v>44228</v>
       </c>
       <c r="B63" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C63">
-        <v>2.5</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
@@ -1181,10 +1184,10 @@
         <v>44256</v>
       </c>
       <c r="B64" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C64">
-        <v>2.54</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
@@ -1192,10 +1195,10 @@
         <v>44287</v>
       </c>
       <c r="B65" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C65">
-        <v>2.4700000000000002</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
@@ -1203,10 +1206,10 @@
         <v>44317</v>
       </c>
       <c r="B66" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C66">
-        <v>2.5</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
@@ -1214,10 +1217,10 @@
         <v>44197</v>
       </c>
       <c r="B67" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C67">
-        <v>0.64</v>
+        <v>2.4900000000000002</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
@@ -1225,10 +1228,10 @@
         <v>44228</v>
       </c>
       <c r="B68" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C68">
-        <v>0.67</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
@@ -1236,10 +1239,10 @@
         <v>44256</v>
       </c>
       <c r="B69" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C69">
-        <v>0.7</v>
+        <v>2.54</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
@@ -1247,10 +1250,10 @@
         <v>44287</v>
       </c>
       <c r="B70" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C70">
-        <v>0.69</v>
+        <v>2.4700000000000002</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
@@ -1258,10 +1261,10 @@
         <v>44317</v>
       </c>
       <c r="B71" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C71">
-        <v>0.61</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
@@ -1269,10 +1272,10 @@
         <v>44197</v>
       </c>
       <c r="B72" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C72">
-        <v>0.1</v>
+        <v>0.64</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
@@ -1280,10 +1283,10 @@
         <v>44228</v>
       </c>
       <c r="B73" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C73">
-        <v>0.11</v>
+        <v>0.67</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
@@ -1291,10 +1294,10 @@
         <v>44256</v>
       </c>
       <c r="B74" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C74">
-        <v>0.13</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
@@ -1302,10 +1305,10 @@
         <v>44287</v>
       </c>
       <c r="B75" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C75">
-        <v>0.14000000000000001</v>
+        <v>0.69</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
@@ -1313,10 +1316,10 @@
         <v>44317</v>
       </c>
       <c r="B76" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C76">
-        <v>0.15</v>
+        <v>0.61</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
@@ -1324,10 +1327,10 @@
         <v>44197</v>
       </c>
       <c r="B77" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C77">
-        <v>0.38</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
@@ -1335,10 +1338,10 @@
         <v>44228</v>
       </c>
       <c r="B78" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C78">
-        <v>0.39</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
@@ -1346,10 +1349,10 @@
         <v>44256</v>
       </c>
       <c r="B79" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C79">
-        <v>0.4</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
@@ -1357,10 +1360,10 @@
         <v>44287</v>
       </c>
       <c r="B80" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C80">
-        <v>0.41</v>
+        <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
@@ -1368,10 +1371,10 @@
         <v>44317</v>
       </c>
       <c r="B81" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C81">
-        <v>0.42</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
@@ -1379,10 +1382,10 @@
         <v>44197</v>
       </c>
       <c r="B82" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C82">
-        <v>0.04</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
@@ -1390,10 +1393,10 @@
         <v>44228</v>
       </c>
       <c r="B83" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C83">
-        <v>0.05</v>
+        <v>0.39</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
@@ -1401,10 +1404,10 @@
         <v>44256</v>
       </c>
       <c r="B84" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C84">
-        <v>0.06</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
@@ -1412,10 +1415,10 @@
         <v>44287</v>
       </c>
       <c r="B85" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C85">
-        <v>0.08</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
@@ -1423,10 +1426,10 @@
         <v>44317</v>
       </c>
       <c r="B86" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C86">
-        <v>0.1</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
@@ -1434,10 +1437,10 @@
         <v>44197</v>
       </c>
       <c r="B87" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C87">
-        <v>0.14000000000000001</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
@@ -1445,10 +1448,10 @@
         <v>44228</v>
       </c>
       <c r="B88" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C88">
-        <v>0.15</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
@@ -1456,10 +1459,10 @@
         <v>44256</v>
       </c>
       <c r="B89" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C89">
-        <v>0.16</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
@@ -1467,10 +1470,10 @@
         <v>44287</v>
       </c>
       <c r="B90" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C90">
-        <v>0.17</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
@@ -1478,10 +1481,10 @@
         <v>44317</v>
       </c>
       <c r="B91" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C91">
-        <v>0.16</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
@@ -1489,10 +1492,10 @@
         <v>44197</v>
       </c>
       <c r="B92" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C92">
-        <v>0.5</v>
+        <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
@@ -1500,10 +1503,10 @@
         <v>44228</v>
       </c>
       <c r="B93" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C93">
-        <v>0.54</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
@@ -1511,10 +1514,10 @@
         <v>44256</v>
       </c>
       <c r="B94" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C94">
-        <v>0.55000000000000004</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
@@ -1522,10 +1525,10 @@
         <v>44287</v>
       </c>
       <c r="B95" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C95">
-        <v>0.55000000000000004</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
@@ -1533,10 +1536,10 @@
         <v>44317</v>
       </c>
       <c r="B96" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C96">
-        <v>0.56999999999999995</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
@@ -1544,10 +1547,10 @@
         <v>44197</v>
       </c>
       <c r="B97" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C97">
-        <v>2.33</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
@@ -1555,10 +1558,10 @@
         <v>44228</v>
       </c>
       <c r="B98" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C98">
-        <v>2.2999999999999998</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.35">
@@ -1566,10 +1569,10 @@
         <v>44256</v>
       </c>
       <c r="B99" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C99">
-        <v>2.36</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.35">
@@ -1577,10 +1580,10 @@
         <v>44287</v>
       </c>
       <c r="B100" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C100">
-        <v>2.4</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.35">
@@ -1588,10 +1591,10 @@
         <v>44317</v>
       </c>
       <c r="B101" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C101">
-        <v>2.31</v>
+        <v>0.56999999999999995</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.35">
@@ -1599,10 +1602,10 @@
         <v>44197</v>
       </c>
       <c r="B102" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C102">
-        <v>1.6</v>
+        <v>2.33</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.35">
@@ -1610,10 +1613,10 @@
         <v>44228</v>
       </c>
       <c r="B103" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C103">
-        <v>1.63</v>
+        <v>2.2999999999999998</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.35">
@@ -1621,10 +1624,10 @@
         <v>44256</v>
       </c>
       <c r="B104" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C104">
-        <v>1.49</v>
+        <v>2.36</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.35">
@@ -1632,10 +1635,10 @@
         <v>44287</v>
       </c>
       <c r="B105" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C105">
-        <v>1.45</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.35">
@@ -1643,10 +1646,10 @@
         <v>44317</v>
       </c>
       <c r="B106" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C106">
-        <v>1.5</v>
+        <v>2.31</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.35">
@@ -1654,10 +1657,10 @@
         <v>44197</v>
       </c>
       <c r="B107" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C107">
-        <v>0.2</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.35">
@@ -1665,10 +1668,10 @@
         <v>44228</v>
       </c>
       <c r="B108" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C108">
-        <v>0.21</v>
+        <v>1.63</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.35">
@@ -1676,10 +1679,10 @@
         <v>44256</v>
       </c>
       <c r="B109" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C109">
-        <v>0.25</v>
+        <v>1.49</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.35">
@@ -1687,10 +1690,10 @@
         <v>44287</v>
       </c>
       <c r="B110" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C110">
-        <v>0.24</v>
+        <v>1.45</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.35">
@@ -1698,10 +1701,10 @@
         <v>44317</v>
       </c>
       <c r="B111" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C111">
-        <v>0.23</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.35">
@@ -1709,10 +1712,10 @@
         <v>44197</v>
       </c>
       <c r="B112" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C112">
-        <v>0.99</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.35">
@@ -1720,10 +1723,10 @@
         <v>44228</v>
       </c>
       <c r="B113" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C113">
-        <v>1</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.35">
@@ -1731,10 +1734,10 @@
         <v>44256</v>
       </c>
       <c r="B114" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C114">
-        <v>0.96</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.35">
@@ -1742,10 +1745,10 @@
         <v>44287</v>
       </c>
       <c r="B115" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C115">
-        <v>0.98</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.35">
@@ -1753,10 +1756,10 @@
         <v>44317</v>
       </c>
       <c r="B116" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C116">
-        <v>1.1000000000000001</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.35">
@@ -1764,10 +1767,10 @@
         <v>44197</v>
       </c>
       <c r="B117" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C117">
-        <v>0.39</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.35">
@@ -1775,10 +1778,10 @@
         <v>44228</v>
       </c>
       <c r="B118" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C118">
-        <v>0.4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.35">
@@ -1786,10 +1789,10 @@
         <v>44256</v>
       </c>
       <c r="B119" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C119">
-        <v>0.4</v>
+        <v>0.96</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.35">
@@ -1797,10 +1800,10 @@
         <v>44287</v>
       </c>
       <c r="B120" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C120">
-        <v>0.41</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.35">
@@ -1808,10 +1811,10 @@
         <v>44317</v>
       </c>
       <c r="B121" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C121">
-        <v>0.42</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.35">
@@ -1819,10 +1822,10 @@
         <v>44197</v>
       </c>
       <c r="B122" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C122">
-        <v>0.11</v>
+        <v>0.39</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.35">
@@ -1830,10 +1833,10 @@
         <v>44228</v>
       </c>
       <c r="B123" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C123">
-        <v>0.15</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.35">
@@ -1841,10 +1844,10 @@
         <v>44256</v>
       </c>
       <c r="B124" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C124">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.35">
@@ -1852,10 +1855,10 @@
         <v>44287</v>
       </c>
       <c r="B125" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C125">
-        <v>0.17</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.35">
@@ -1863,10 +1866,10 @@
         <v>44317</v>
       </c>
       <c r="B126" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C126">
-        <v>0.18</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.35">
@@ -1874,10 +1877,10 @@
         <v>44197</v>
       </c>
       <c r="B127" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C127">
-        <v>3.61</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.35">
@@ -1885,10 +1888,10 @@
         <v>44228</v>
       </c>
       <c r="B128" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C128">
-        <v>3.55</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.35">
@@ -1896,10 +1899,10 @@
         <v>44256</v>
       </c>
       <c r="B129" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C129">
-        <v>3.73</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.35">
@@ -1907,10 +1910,10 @@
         <v>44287</v>
       </c>
       <c r="B130" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C130">
-        <v>3.71</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.35">
@@ -1918,10 +1921,10 @@
         <v>44317</v>
       </c>
       <c r="B131" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C131">
-        <v>3.6</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.35">
@@ -1929,10 +1932,10 @@
         <v>44197</v>
       </c>
       <c r="B132" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C132">
-        <v>0.92</v>
+        <v>3.61</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.35">
@@ -1940,10 +1943,10 @@
         <v>44228</v>
       </c>
       <c r="B133" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C133">
-        <v>0.95</v>
+        <v>3.55</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.35">
@@ -1951,10 +1954,10 @@
         <v>44256</v>
       </c>
       <c r="B134" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C134">
-        <v>1</v>
+        <v>3.73</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.35">
@@ -1962,10 +1965,10 @@
         <v>44287</v>
       </c>
       <c r="B135" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C135">
-        <v>0.99</v>
+        <v>3.71</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.35">
@@ -1973,10 +1976,10 @@
         <v>44317</v>
       </c>
       <c r="B136" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C136">
-        <v>0.99</v>
+        <v>3.6</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.35">
@@ -1984,10 +1987,10 @@
         <v>44197</v>
       </c>
       <c r="B137" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C137">
-        <v>1.4</v>
+        <v>0.92</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.35">
@@ -1995,10 +1998,10 @@
         <v>44228</v>
       </c>
       <c r="B138" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C138">
-        <v>1.46</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.35">
@@ -2006,10 +2009,10 @@
         <v>44256</v>
       </c>
       <c r="B139" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C139">
-        <v>1.48</v>
+        <v>1</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.35">
@@ -2017,10 +2020,10 @@
         <v>44287</v>
       </c>
       <c r="B140" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C140">
-        <v>1.49</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.35">
@@ -2028,26 +2031,66 @@
         <v>44317</v>
       </c>
       <c r="B141" t="s">
+        <v>28</v>
+      </c>
+      <c r="C141">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A142" s="1">
+        <v>44197</v>
+      </c>
+      <c r="B142" t="s">
         <v>29</v>
       </c>
-      <c r="C141">
+      <c r="C142">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A143" s="1">
+        <v>44228</v>
+      </c>
+      <c r="B143" t="s">
+        <v>29</v>
+      </c>
+      <c r="C143">
+        <v>1.46</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A144" s="1">
+        <v>44256</v>
+      </c>
+      <c r="B144" t="s">
+        <v>29</v>
+      </c>
+      <c r="C144">
+        <v>1.48</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A145" s="1">
+        <v>44287</v>
+      </c>
+      <c r="B145" t="s">
+        <v>29</v>
+      </c>
+      <c r="C145">
+        <v>1.49</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A146" s="1">
+        <v>44317</v>
+      </c>
+      <c r="B146" t="s">
+        <v>29</v>
+      </c>
+      <c r="C146">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A142" s="1"/>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A143" s="1"/>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A144" s="1"/>
-    </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A145" s="1"/>
-    </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A146" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>